<commit_message>
Started EMP removal + major/minor action revamp
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/AllSpells.xlsx
+++ b/CoreRulebook/Data/Spells/AllSpells.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="1081">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -4015,37 +4015,8 @@
   </si>
   <si>
     <t xml:space="preserve">Erects an ethereal shield from your in front of you that absorbs incoming magical attacks.
-Shielding charm provides a magical AC by 10+PP against all incoming spells, but does not protect against physical damage, or the aftereffects of magic (i.e. a nearby explosion). This AC is eroded by all damage-causing effects.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">When cast by a character greater than 10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> level, the AC provided is equal to the character level + $2 \times PP$.</t>
-    </r>
+Casting this spell initiates a `Brace’ action and, in addition to the Resist check, adds (1d4 +PP) to your Block stat against magical attacks. 
+This shield has a health of (10 +$5\times$PP). If a spell would cause the shield to drop to 0HP, the shield fails, and half the remaining damage is dealt to the caster. </t>
   </si>
   <si>
     <t xml:space="preserve">Magical Stability Ward</t>
@@ -4063,37 +4034,7 @@
     <t xml:space="preserve">tueormaxima</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual Ward (see Lesser Ward) that protects against 50 damage. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">When cast by a character greater than 14</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> level, the ward protection is equal to four times the character level. </t>
-    </r>
+    <t xml:space="preserve">Individual Ward (see Lesser Ward) that protects against (50+5$\times$PP) damage. </t>
   </si>
   <si>
     <t xml:space="preserve">Minefield Ward</t>
@@ -4111,7 +4052,10 @@
     <t xml:space="preserve">repente</t>
   </si>
   <si>
-    <t xml:space="preserve">A more powerful version of the shielding charm (see protego for full description) with AC 25+$2\times$PP, but rather than spells being absorbed by the shield, they are reflected back at the caster. Mirror shield also defends against physical attacks.</t>
+    <t xml:space="preserve">Erects an ethereal shield from your in front of you that absorbs incoming attacks of all kinds.
+Casting this spell initiates a `Brace’ action and, in addition to the Resist check, adds (1d4 +PP) to your Block stat against magical and physical attacks. 
+This shield has a health of (10 +$5\times$PP). If a spell would cause the shield to drop to 0HP, the shield fails, and half the remaining damage is dealt to the caster. 
+On a successful block of a spell that the caster knows, they may perform an accuracy check to `reflect\apos{} the spell back at the original caster. This costs no additional FP to do, and on a failed attempt, the spell is reflected in a random direction. Reflected spells still drain the shield\apos{}s HP. </t>
   </si>
   <si>
     <t xml:space="preserve">Privacy Ward</t>
@@ -4120,7 +4064,7 @@
     <t xml:space="preserve">muffliato</t>
   </si>
   <si>
-    <t xml:space="preserve">A buzzing sound fills the ears of anyone trying to listen in on your conversations whilst you are in the warded area. Lasts for one hour, and has a radius of 2m.</t>
+    <t xml:space="preserve">Prevents sound from inside a region (2+PP)m in radius being heard from the outside. When inside the region, sound from both inside and outside may be heard. </t>
   </si>
   <si>
     <t xml:space="preserve">Reinforce Shield</t>
@@ -4168,37 +4112,15 @@
     <t xml:space="preserve">1 year</t>
   </si>
   <si>
-    <t xml:space="preserve">Prevents objects from passing over the edge of the ward. Usually cast on doorways and entrances. The ward is immune to all physical damage, but can only survive 8 points of spell damage. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">When cast by a character greater than 12</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="aakar"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> level, ward strength is equal to character level. </t>
-    </r>
+    <t xml:space="preserve">Prevents objects from passing over the edge of the ward. Usually cast on doorways and entrances. The ward is immune to all physical damage, but can only survive (8+$2\times$PP) points of spell damage. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apparate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may teleport yourself and up to PP additional passengers to a place you are intimitaely familiar with. Passengers must be in physical contact with you the moment this spell is cast. 
+This spell may be cast without the use of a wand. 
+If anything happens to the caster in the turn that this spell is cast which would disrupt a Focus spell, all passengers become splinched and take 2d12 force damage. </t>
   </si>
 </sst>
 </file>
@@ -4503,12 +4425,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -4582,34 +4504,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:GD273"/>
+  <dimension ref="A1:GD274"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
-      <selection pane="bottomRight" activeCell="I88" activeCellId="0" sqref="I88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="B263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="L269" activeCellId="0" sqref="L269"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="55.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="36.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="16" style="1" width="4.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="38" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="5.01"/>
@@ -4617,19 +4537,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="68" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="1" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="84" style="2" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="2" width="4.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="104" min="104" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="105" style="1" width="2.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="125" min="125" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="126" style="1" width="4.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="185" min="167" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="167" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="1" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="187" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="187" style="1" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -41627,7 +41547,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="78.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="11" t="s">
         <v>1044</v>
       </c>
@@ -41658,13 +41578,11 @@
       <c r="L264" s="11" t="s">
         <v>1047</v>
       </c>
-      <c r="M264" s="19" t="s">
-        <v>1048</v>
-      </c>
+      <c r="M264" s="19"/>
     </row>
     <row r="265" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>453</v>
@@ -41673,7 +41591,7 @@
         <v>1002</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E265" s="1" t="s">
         <v>359</v>
@@ -41688,12 +41606,12 @@
         <v>5</v>
       </c>
       <c r="L265" s="1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="11" t="s">
         <v>1051</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="11" t="s">
-        <v>1052</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>453</v>
@@ -41702,7 +41620,7 @@
         <v>1002</v>
       </c>
       <c r="D266" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E266" s="11" t="s">
         <v>359</v>
@@ -41720,15 +41638,13 @@
       <c r="J266" s="11"/>
       <c r="K266" s="11"/>
       <c r="L266" s="11" t="s">
-        <v>1054</v>
-      </c>
-      <c r="M266" s="19" t="s">
-        <v>1055</v>
-      </c>
+        <v>1053</v>
+      </c>
+      <c r="M266" s="19"/>
     </row>
     <row r="267" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="11" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>453</v>
@@ -41737,7 +41653,7 @@
         <v>1002</v>
       </c>
       <c r="D267" s="11" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E267" s="11" t="s">
         <v>359</v>
@@ -41759,7 +41675,7 @@
         <v>10</v>
       </c>
       <c r="L267" s="11" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="N267" s="1" t="n">
         <v>1</v>
@@ -42254,9 +42170,9 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="169.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="11" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>453</v>
@@ -42265,7 +42181,7 @@
         <v>1002</v>
       </c>
       <c r="D268" s="11" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="E268" s="11" t="s">
         <v>98</v>
@@ -42283,12 +42199,12 @@
       <c r="J268" s="11"/>
       <c r="K268" s="11"/>
       <c r="L268" s="11" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="11" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>453</v>
@@ -42297,7 +42213,7 @@
         <v>1002</v>
       </c>
       <c r="D269" s="11" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E269" s="11" t="s">
         <v>359</v>
@@ -42315,12 +42231,12 @@
       <c r="J269" s="11"/>
       <c r="K269" s="11"/>
       <c r="L269" s="11" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="11" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>453</v>
@@ -42329,7 +42245,7 @@
         <v>1002</v>
       </c>
       <c r="D270" s="11" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E270" s="11" t="s">
         <v>98</v>
@@ -42338,7 +42254,7 @@
         <v>59</v>
       </c>
       <c r="G270" s="11" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="H270" s="11"/>
       <c r="I270" s="11" t="n">
@@ -42347,15 +42263,15 @@
       <c r="J270" s="11"/>
       <c r="K270" s="11"/>
       <c r="L270" s="11" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="M270" s="1" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="11" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>453</v>
@@ -42364,7 +42280,7 @@
         <v>1002</v>
       </c>
       <c r="D271" s="11" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E271" s="11" t="s">
         <v>29</v>
@@ -42373,7 +42289,7 @@
         <v>59</v>
       </c>
       <c r="G271" s="11" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="H271" s="11" t="s">
         <v>31</v>
@@ -42384,12 +42300,12 @@
       <c r="J271" s="11"/>
       <c r="K271" s="11"/>
       <c r="L271" s="11" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>453</v>
@@ -42398,7 +42314,7 @@
         <v>1002</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="E272" s="1" t="s">
         <v>98</v>
@@ -42410,15 +42326,15 @@
         <v>946</v>
       </c>
       <c r="I272" s="11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L272" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="11" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>453</v>
@@ -42427,7 +42343,7 @@
         <v>1002</v>
       </c>
       <c r="D273" s="11" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E273" s="11" t="s">
         <v>359</v>
@@ -42437,7 +42353,7 @@
       </c>
       <c r="G273" s="11"/>
       <c r="H273" s="11" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="I273" s="11" t="n">
         <v>3</v>
@@ -42445,10 +42361,31 @@
       <c r="J273" s="11"/>
       <c r="K273" s="11"/>
       <c r="L273" s="11" t="s">
+        <v>1078</v>
+      </c>
+      <c r="M273" s="19"/>
+    </row>
+    <row r="274" customFormat="false" ht="95.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I274" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L274" s="1" t="s">
         <v>1080</v>
-      </c>
-      <c r="M273" s="19" t="s">
-        <v>1081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lilly potter spell added
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/AllSpells.xlsx
+++ b/CoreRulebook/Data/Spells/AllSpells.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="1037">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -3351,6 +3351,14 @@
   <si>
     <t xml:space="preserve">If the spell makes contact with the target, kills them instantly. 
 When encountering shields and other protective barriers, deals 10d10 damage to them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sacrifice\apos{}s Shield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You allow the next strike made against you to kill you, and banish your soul to the Eldritch domains. In return, your sacrifice and love fuels a charm so powerful it cannot be resisted or overcome by force alone. 
+You may nominate an individual sapient being. That individual cannot be harmed by the being which killed you. Any attempt by your killer to harm your nominated individual simply reflects the charm back upon you. 
+This spell does not need a casting check to cast. </t>
   </si>
 </sst>
 </file>
@@ -3722,14 +3730,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:FK278"/>
+  <dimension ref="A1:FK279"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E273" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A273" activeCellId="0" sqref="A273"/>
-      <selection pane="bottomRight" activeCell="L281" activeCellId="0" sqref="L281"/>
+      <selection pane="bottomRight" activeCell="L279" activeCellId="0" sqref="L279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22821,6 +22829,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="279" customFormat="false" ht="94.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D279" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L279" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:EP292"/>
   <mergeCells count="19">

</xml_diff>

<commit_message>
Diagon alley map added +new potion system introduced
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/AllSpells.xlsx
+++ b/CoreRulebook/Data/Spells/AllSpells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Spells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4700EF50-9426-4130-BD79-E57CC0C5AEFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26AABCC-CD75-4299-BE30-79E504B47718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3055,14 +3055,6 @@
     <t>protego</t>
   </si>
   <si>
-    <t xml:space="preserve">This spell erects an impenetrable, ethereal shield in front of the caster which absorbs incoming attacks.
-This shield has a health of 10HP. If an attack is blocked which would cause the shield to drop to 0HP, the shield fails, and half the remaining damage is dealt to the caster. 
-The caster is not considered {\it Distracted} when casting this spell, unless attacked by an enemy that they cannot see. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The HP of the shield doubles for every additional spell level used to cast the shield </t>
-  </si>
-  <si>
     <t>Privacy Ward</t>
   </si>
   <si>
@@ -4146,6 +4138,15 @@
   </si>
   <si>
     <t xml:space="preserve">Target a sapient being, on a failed Resist, the caster is notified by a glowing aura and a soft chime whenever the target makes a statement which they know to be false. The target is unaware of the casting of this spell unless they pass a DV 15 Observation check. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An ethereal shield blossoms from the end of your wand, protecting you from both magical and physical harm. 
+Whenever an attack is performed against you whilst the shield is active, roll 2d4 and add this value to your Resist check or your Block value, as appropriate. If a successful Resist would limit the amount of damage taken, negate it entirely instead. 
+If you fail to Resist, or the Accuracy exceeds your augmented Block value, the shield crumples and the spell is ended. The spell which broke the shield is then applied to you at half damage, with any other effects unmodified. Any other spells which hit you this round act as normal. 
+The caster is not considered {\it Distracted} when casting this spell, unless attacked by an enemy that they cannot see. </t>
+  </si>
+  <si>
+    <t>Increase the strength of the shield by 1 point \forEvery{}.</t>
   </si>
 </sst>
 </file>
@@ -4356,13 +4357,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4750,10 +4751,10 @@
   <dimension ref="A1:AMK342"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="K251" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="A117" sqref="A117"/>
+      <selection pane="bottomRight" activeCell="L253" sqref="L253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -4791,46 +4792,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:167" s="6" customFormat="1" ht="24">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="25" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -4932,8 +4933,8 @@
       <c r="BY1" s="5"/>
       <c r="BZ1" s="5"/>
       <c r="CA1" s="5"/>
-      <c r="CC1" s="24"/>
-      <c r="CE1" s="23"/>
+      <c r="CC1" s="25"/>
+      <c r="CE1" s="24"/>
       <c r="CF1" s="7"/>
       <c r="CG1" s="8"/>
       <c r="CH1" s="8"/>
@@ -4955,82 +4956,82 @@
       <c r="CX1" s="8"/>
       <c r="CY1" s="8"/>
       <c r="CZ1" s="9"/>
-      <c r="DB1" s="24"/>
-      <c r="DC1" s="24"/>
-      <c r="DD1" s="24"/>
-      <c r="DE1" s="24"/>
-      <c r="DF1" s="24"/>
-      <c r="DG1" s="24"/>
-      <c r="DH1" s="24"/>
-      <c r="DI1" s="24"/>
-      <c r="DJ1" s="24"/>
-      <c r="DK1" s="24"/>
-      <c r="DL1" s="24"/>
-      <c r="DM1" s="24"/>
-      <c r="DN1" s="24"/>
-      <c r="DO1" s="24"/>
-      <c r="DP1" s="24"/>
-      <c r="DQ1" s="24"/>
-      <c r="DR1" s="24"/>
-      <c r="DS1" s="24"/>
-      <c r="DT1" s="24"/>
-      <c r="DU1" s="24"/>
-      <c r="DW1" s="24"/>
-      <c r="DX1" s="24"/>
-      <c r="DY1" s="24"/>
-      <c r="DZ1" s="24"/>
-      <c r="EA1" s="24"/>
-      <c r="EB1" s="24"/>
-      <c r="EC1" s="24"/>
-      <c r="ED1" s="24"/>
-      <c r="EE1" s="24"/>
-      <c r="EF1" s="24"/>
-      <c r="EG1" s="24"/>
-      <c r="EH1" s="24"/>
-      <c r="EI1" s="24"/>
-      <c r="EJ1" s="24"/>
-      <c r="EK1" s="24"/>
-      <c r="EL1" s="24"/>
-      <c r="EM1" s="24"/>
-      <c r="EN1" s="24"/>
-      <c r="EO1" s="24"/>
-      <c r="EP1" s="24"/>
-      <c r="ER1" s="24"/>
-      <c r="ES1" s="24"/>
-      <c r="ET1" s="24"/>
-      <c r="EU1" s="24"/>
-      <c r="EV1" s="24"/>
-      <c r="EW1" s="24"/>
-      <c r="EX1" s="24"/>
-      <c r="EY1" s="24"/>
-      <c r="EZ1" s="24"/>
-      <c r="FA1" s="24"/>
-      <c r="FB1" s="24"/>
-      <c r="FC1" s="24"/>
-      <c r="FD1" s="24"/>
-      <c r="FE1" s="24"/>
-      <c r="FF1" s="24"/>
-      <c r="FG1" s="24"/>
-      <c r="FH1" s="24"/>
-      <c r="FI1" s="24"/>
-      <c r="FJ1" s="24"/>
-      <c r="FK1" s="24"/>
+      <c r="DB1" s="25"/>
+      <c r="DC1" s="25"/>
+      <c r="DD1" s="25"/>
+      <c r="DE1" s="25"/>
+      <c r="DF1" s="25"/>
+      <c r="DG1" s="25"/>
+      <c r="DH1" s="25"/>
+      <c r="DI1" s="25"/>
+      <c r="DJ1" s="25"/>
+      <c r="DK1" s="25"/>
+      <c r="DL1" s="25"/>
+      <c r="DM1" s="25"/>
+      <c r="DN1" s="25"/>
+      <c r="DO1" s="25"/>
+      <c r="DP1" s="25"/>
+      <c r="DQ1" s="25"/>
+      <c r="DR1" s="25"/>
+      <c r="DS1" s="25"/>
+      <c r="DT1" s="25"/>
+      <c r="DU1" s="25"/>
+      <c r="DW1" s="25"/>
+      <c r="DX1" s="25"/>
+      <c r="DY1" s="25"/>
+      <c r="DZ1" s="25"/>
+      <c r="EA1" s="25"/>
+      <c r="EB1" s="25"/>
+      <c r="EC1" s="25"/>
+      <c r="ED1" s="25"/>
+      <c r="EE1" s="25"/>
+      <c r="EF1" s="25"/>
+      <c r="EG1" s="25"/>
+      <c r="EH1" s="25"/>
+      <c r="EI1" s="25"/>
+      <c r="EJ1" s="25"/>
+      <c r="EK1" s="25"/>
+      <c r="EL1" s="25"/>
+      <c r="EM1" s="25"/>
+      <c r="EN1" s="25"/>
+      <c r="EO1" s="25"/>
+      <c r="EP1" s="25"/>
+      <c r="ER1" s="25"/>
+      <c r="ES1" s="25"/>
+      <c r="ET1" s="25"/>
+      <c r="EU1" s="25"/>
+      <c r="EV1" s="25"/>
+      <c r="EW1" s="25"/>
+      <c r="EX1" s="25"/>
+      <c r="EY1" s="25"/>
+      <c r="EZ1" s="25"/>
+      <c r="FA1" s="25"/>
+      <c r="FB1" s="25"/>
+      <c r="FC1" s="25"/>
+      <c r="FD1" s="25"/>
+      <c r="FE1" s="25"/>
+      <c r="FF1" s="25"/>
+      <c r="FG1" s="25"/>
+      <c r="FH1" s="25"/>
+      <c r="FI1" s="25"/>
+      <c r="FJ1" s="25"/>
+      <c r="FK1" s="25"/>
     </row>
     <row r="2" spans="1:167" s="6" customFormat="1" ht="18">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
@@ -5125,9 +5126,9 @@
       <c r="BZ2" s="10"/>
       <c r="CA2" s="10"/>
       <c r="CB2" s="10"/>
-      <c r="CC2" s="24"/>
+      <c r="CC2" s="25"/>
       <c r="CD2" s="10"/>
-      <c r="CE2" s="23"/>
+      <c r="CE2" s="24"/>
       <c r="CF2" s="10"/>
       <c r="CG2" s="10"/>
       <c r="CH2" s="10"/>
@@ -5150,7 +5151,7 @@
       <c r="CY2" s="8"/>
       <c r="CZ2" s="9"/>
     </row>
-    <row r="3" spans="1:167" ht="36">
+    <row r="3" spans="1:167" ht="24">
       <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
@@ -5233,7 +5234,7 @@
       <c r="CE3" s="2"/>
       <c r="CF3" s="2"/>
     </row>
-    <row r="4" spans="1:167" ht="216">
+    <row r="4" spans="1:167" ht="192">
       <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:167" ht="156">
+    <row r="5" spans="1:167" ht="132">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -5652,7 +5653,7 @@
       <c r="CE9" s="2"/>
       <c r="CF9" s="2"/>
     </row>
-    <row r="10" spans="1:167" ht="36">
+    <row r="10" spans="1:167" ht="24">
       <c r="A10" s="11" t="s">
         <v>59</v>
       </c>
@@ -5953,7 +5954,7 @@
       <c r="CE13" s="2"/>
       <c r="CF13" s="2"/>
     </row>
-    <row r="14" spans="1:167" ht="24">
+    <row r="14" spans="1:167">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
@@ -5988,7 +5989,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:167" ht="72">
+    <row r="15" spans="1:167" ht="60">
       <c r="A15" s="13" t="s">
         <v>78</v>
       </c>
@@ -6071,7 +6072,7 @@
       <c r="CE15" s="2"/>
       <c r="CF15" s="2"/>
     </row>
-    <row r="16" spans="1:167" ht="60">
+    <row r="16" spans="1:167" ht="48">
       <c r="A16" s="11" t="s">
         <v>82</v>
       </c>
@@ -6136,7 +6137,7 @@
       <c r="CE16" s="2"/>
       <c r="CF16" s="2"/>
     </row>
-    <row r="17" spans="1:84" ht="36">
+    <row r="17" spans="1:84" ht="24">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -6422,7 +6423,7 @@
       <c r="CE21" s="2"/>
       <c r="CF21" s="2"/>
     </row>
-    <row r="22" spans="1:84" ht="72">
+    <row r="22" spans="1:84" ht="60">
       <c r="A22" s="11" t="s">
         <v>109</v>
       </c>
@@ -6511,7 +6512,7 @@
       <c r="CE22" s="2"/>
       <c r="CF22" s="2"/>
     </row>
-    <row r="23" spans="1:84" ht="48">
+    <row r="23" spans="1:84" ht="36">
       <c r="A23" s="11" t="s">
         <v>113</v>
       </c>
@@ -6540,7 +6541,7 @@
         <v>116</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>117</v>
@@ -6596,7 +6597,7 @@
       <c r="CE23" s="2"/>
       <c r="CF23" s="2"/>
     </row>
-    <row r="24" spans="1:84" ht="72">
+    <row r="24" spans="1:84" ht="60">
       <c r="A24" s="11" t="s">
         <v>118</v>
       </c>
@@ -6745,7 +6746,7 @@
       <c r="CE25" s="2"/>
       <c r="CF25" s="2"/>
     </row>
-    <row r="26" spans="1:84" ht="36">
+    <row r="26" spans="1:84" ht="24">
       <c r="A26" s="11" t="s">
         <v>125</v>
       </c>
@@ -6897,7 +6898,7 @@
       <c r="CE27" s="2"/>
       <c r="CF27" s="2"/>
     </row>
-    <row r="28" spans="1:84" ht="60">
+    <row r="28" spans="1:84" ht="36">
       <c r="A28" s="11" t="s">
         <v>134</v>
       </c>
@@ -6964,7 +6965,7 @@
       <c r="CE28" s="2"/>
       <c r="CF28" s="2"/>
     </row>
-    <row r="29" spans="1:84" ht="48">
+    <row r="29" spans="1:84" ht="36">
       <c r="A29" s="11" t="s">
         <v>139</v>
       </c>
@@ -7114,7 +7115,7 @@
       <c r="CE30" s="2"/>
       <c r="CF30" s="2"/>
     </row>
-    <row r="31" spans="1:84" ht="72">
+    <row r="31" spans="1:84" ht="60">
       <c r="A31" s="11" t="s">
         <v>147</v>
       </c>
@@ -7294,7 +7295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:84" ht="24">
+    <row r="34" spans="1:84">
       <c r="A34" s="11" t="s">
         <v>157</v>
       </c>
@@ -7466,7 +7467,7 @@
       <c r="CE35" s="2"/>
       <c r="CF35" s="2"/>
     </row>
-    <row r="36" spans="1:84" ht="48">
+    <row r="36" spans="1:84" ht="36">
       <c r="A36" s="1" t="s">
         <v>165</v>
       </c>
@@ -7498,7 +7499,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:84" ht="84">
+    <row r="37" spans="1:84" ht="60">
       <c r="A37" s="15" t="s">
         <v>169</v>
       </c>
@@ -7718,7 +7719,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:84" ht="72">
+    <row r="41" spans="1:84" ht="60">
       <c r="A41" s="11" t="s">
         <v>181</v>
       </c>
@@ -7900,7 +7901,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:84" ht="120">
+    <row r="44" spans="1:84" ht="108">
       <c r="A44" s="11" t="s">
         <v>190</v>
       </c>
@@ -8283,7 +8284,7 @@
       <c r="CE49" s="2"/>
       <c r="CF49" s="2"/>
     </row>
-    <row r="50" spans="1:84" ht="60">
+    <row r="50" spans="1:84" ht="48">
       <c r="A50" s="11" t="s">
         <v>211</v>
       </c>
@@ -8477,7 +8478,7 @@
       <c r="CE52" s="2"/>
       <c r="CF52" s="2"/>
     </row>
-    <row r="53" spans="1:84" ht="36">
+    <row r="53" spans="1:84" ht="24">
       <c r="A53" s="11" t="s">
         <v>221</v>
       </c>
@@ -8632,7 +8633,7 @@
       <c r="CE55" s="2"/>
       <c r="CF55" s="2"/>
     </row>
-    <row r="56" spans="1:84" ht="96">
+    <row r="56" spans="1:84" ht="84">
       <c r="A56" s="1" t="s">
         <v>230</v>
       </c>
@@ -8917,7 +8918,7 @@
       <c r="CE60" s="2"/>
       <c r="CF60" s="2"/>
     </row>
-    <row r="61" spans="1:84" ht="36">
+    <row r="61" spans="1:84" ht="24">
       <c r="A61" s="11" t="s">
         <v>247</v>
       </c>
@@ -9043,7 +9044,7 @@
       <c r="CE62" s="2"/>
       <c r="CF62" s="2"/>
     </row>
-    <row r="63" spans="1:84" ht="36">
+    <row r="63" spans="1:84" ht="24">
       <c r="A63" s="11" t="s">
         <v>253</v>
       </c>
@@ -9398,7 +9399,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:84" ht="72">
+    <row r="69" spans="1:84" ht="60">
       <c r="A69" s="11" t="s">
         <v>279</v>
       </c>
@@ -9605,7 +9606,7 @@
       <c r="CE71" s="2"/>
       <c r="CF71" s="2"/>
     </row>
-    <row r="72" spans="1:84" ht="120">
+    <row r="72" spans="1:84" ht="108">
       <c r="A72" s="11" t="s">
         <v>289</v>
       </c>
@@ -9660,7 +9661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:84" ht="84">
+    <row r="73" spans="1:84" ht="72">
       <c r="A73" s="11" t="s">
         <v>292</v>
       </c>
@@ -9947,7 +9948,7 @@
       <c r="CE76" s="2"/>
       <c r="CF76" s="2"/>
     </row>
-    <row r="77" spans="1:84" ht="36">
+    <row r="77" spans="1:84" ht="24">
       <c r="A77" s="11" t="s">
         <v>310</v>
       </c>
@@ -10032,7 +10033,7 @@
       <c r="CE77" s="2"/>
       <c r="CF77" s="2"/>
     </row>
-    <row r="78" spans="1:84" ht="49.5">
+    <row r="78" spans="1:84" ht="37.5">
       <c r="A78" s="13" t="s">
         <v>314</v>
       </c>
@@ -10182,7 +10183,7 @@
       <c r="CE79" s="2"/>
       <c r="CF79" s="2"/>
     </row>
-    <row r="80" spans="1:84" ht="72">
+    <row r="80" spans="1:84" ht="60">
       <c r="A80" s="13" t="s">
         <v>321</v>
       </c>
@@ -10309,7 +10310,7 @@
       <c r="CE81" s="2"/>
       <c r="CF81" s="2"/>
     </row>
-    <row r="82" spans="1:84" ht="48">
+    <row r="82" spans="1:84" ht="36">
       <c r="A82" s="11" t="s">
         <v>328</v>
       </c>
@@ -10371,7 +10372,7 @@
       <c r="CE82" s="2"/>
       <c r="CF82" s="2"/>
     </row>
-    <row r="83" spans="1:84" ht="84">
+    <row r="83" spans="1:84" ht="72">
       <c r="A83" s="13" t="s">
         <v>331</v>
       </c>
@@ -10460,7 +10461,7 @@
       <c r="CE83" s="2"/>
       <c r="CF83" s="2"/>
     </row>
-    <row r="84" spans="1:84" ht="36">
+    <row r="84" spans="1:84" ht="24">
       <c r="A84" s="11" t="s">
         <v>335</v>
       </c>
@@ -10695,7 +10696,7 @@
       <c r="CE86" s="2"/>
       <c r="CF86" s="2"/>
     </row>
-    <row r="87" spans="1:84" ht="48">
+    <row r="87" spans="1:84" ht="36">
       <c r="A87" s="11" t="s">
         <v>347</v>
       </c>
@@ -10761,7 +10762,7 @@
       <c r="CE87" s="2"/>
       <c r="CF87" s="2"/>
     </row>
-    <row r="88" spans="1:84" ht="192">
+    <row r="88" spans="1:84" ht="168">
       <c r="A88" s="11" t="s">
         <v>351</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:84" ht="132">
+    <row r="91" spans="1:84" ht="108">
       <c r="A91" s="11" t="s">
         <v>362</v>
       </c>
@@ -11250,7 +11251,7 @@
       <c r="CE95" s="2"/>
       <c r="CF95" s="2"/>
     </row>
-    <row r="96" spans="1:84" ht="48">
+    <row r="96" spans="1:84" ht="36">
       <c r="A96" s="13" t="s">
         <v>376</v>
       </c>
@@ -11470,7 +11471,7 @@
       <c r="CE98" s="2"/>
       <c r="CF98" s="2"/>
     </row>
-    <row r="99" spans="1:84" ht="48">
+    <row r="99" spans="1:84" ht="36">
       <c r="A99" s="11" t="s">
         <v>387</v>
       </c>
@@ -11594,7 +11595,7 @@
       <c r="CE100" s="2"/>
       <c r="CF100" s="2"/>
     </row>
-    <row r="101" spans="1:84" ht="36">
+    <row r="101" spans="1:84" ht="24">
       <c r="A101" s="13" t="s">
         <v>393</v>
       </c>
@@ -11886,7 +11887,7 @@
       <c r="CE104" s="2"/>
       <c r="CF104" s="2"/>
     </row>
-    <row r="105" spans="1:84" ht="48">
+    <row r="105" spans="1:84" ht="36">
       <c r="A105" s="11" t="s">
         <v>407</v>
       </c>
@@ -11946,7 +11947,7 @@
       <c r="CE105" s="2"/>
       <c r="CF105" s="2"/>
     </row>
-    <row r="106" spans="1:84" ht="132">
+    <row r="106" spans="1:84" ht="120">
       <c r="A106" s="11" t="s">
         <v>409</v>
       </c>
@@ -12407,7 +12408,7 @@
       <c r="CE113" s="2"/>
       <c r="CF113" s="2"/>
     </row>
-    <row r="114" spans="1:84" ht="84">
+    <row r="114" spans="1:84" ht="72">
       <c r="A114" s="11" t="s">
         <v>441</v>
       </c>
@@ -12469,7 +12470,7 @@
       <c r="CE114" s="2"/>
       <c r="CF114" s="2"/>
     </row>
-    <row r="115" spans="1:84" ht="120">
+    <row r="115" spans="1:84" ht="108">
       <c r="A115" s="11" t="s">
         <v>444</v>
       </c>
@@ -12661,7 +12662,7 @@
       <c r="CE117" s="2"/>
       <c r="CF117" s="2"/>
     </row>
-    <row r="118" spans="1:84" ht="24">
+    <row r="118" spans="1:84">
       <c r="A118" s="11" t="s">
         <v>456</v>
       </c>
@@ -12723,7 +12724,7 @@
       <c r="CE118" s="2"/>
       <c r="CF118" s="2"/>
     </row>
-    <row r="119" spans="1:84" ht="60">
+    <row r="119" spans="1:84" ht="48">
       <c r="A119" s="11" t="s">
         <v>459</v>
       </c>
@@ -13154,7 +13155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:84" ht="120">
+    <row r="126" spans="1:84" ht="96">
       <c r="A126" s="11" t="s">
         <v>482</v>
       </c>
@@ -13274,7 +13275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:84" ht="36">
+    <row r="128" spans="1:84" ht="24">
       <c r="A128" s="11" t="s">
         <v>489</v>
       </c>
@@ -13333,7 +13334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:84" ht="120">
+    <row r="129" spans="1:84" ht="108">
       <c r="A129" s="11" t="s">
         <v>493</v>
       </c>
@@ -13526,7 +13527,7 @@
       <c r="CE131" s="2"/>
       <c r="CF131" s="2"/>
     </row>
-    <row r="132" spans="1:84" ht="120">
+    <row r="132" spans="1:84" ht="84">
       <c r="A132" s="11" t="s">
         <v>504</v>
       </c>
@@ -13640,7 +13641,7 @@
       <c r="CE133" s="2"/>
       <c r="CF133" s="2"/>
     </row>
-    <row r="134" spans="1:84" ht="72">
+    <row r="134" spans="1:84" ht="60">
       <c r="A134" s="11" t="s">
         <v>509</v>
       </c>
@@ -13702,7 +13703,7 @@
       <c r="CE134" s="2"/>
       <c r="CF134" s="2"/>
     </row>
-    <row r="135" spans="1:84" ht="48">
+    <row r="135" spans="1:84" ht="36">
       <c r="A135" s="11" t="s">
         <v>512</v>
       </c>
@@ -14197,7 +14198,7 @@
       <c r="CE141" s="2"/>
       <c r="CF141" s="2"/>
     </row>
-    <row r="142" spans="1:84" ht="120">
+    <row r="142" spans="1:84" ht="96">
       <c r="A142" s="11" t="s">
         <v>540</v>
       </c>
@@ -14233,7 +14234,7 @@
       <c r="CE142" s="2"/>
       <c r="CF142" s="2"/>
     </row>
-    <row r="143" spans="1:84" ht="36">
+    <row r="143" spans="1:84" ht="24">
       <c r="A143" s="11" t="s">
         <v>542</v>
       </c>
@@ -14363,7 +14364,7 @@
       <c r="CE144" s="2"/>
       <c r="CF144" s="2"/>
     </row>
-    <row r="145" spans="1:84" ht="60">
+    <row r="145" spans="1:84" ht="48">
       <c r="A145" s="11" t="s">
         <v>550</v>
       </c>
@@ -14536,7 +14537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:84" ht="72">
+    <row r="148" spans="1:84" ht="60">
       <c r="A148" s="1" t="s">
         <v>559</v>
       </c>
@@ -14589,7 +14590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:84" ht="204">
+    <row r="149" spans="1:84" ht="180">
       <c r="A149" s="13" t="s">
         <v>562</v>
       </c>
@@ -14651,7 +14652,7 @@
       <c r="CE149" s="2"/>
       <c r="CF149" s="2"/>
     </row>
-    <row r="150" spans="1:84" ht="120">
+    <row r="150" spans="1:84" ht="108">
       <c r="A150" s="11" t="s">
         <v>565</v>
       </c>
@@ -14689,7 +14690,7 @@
       <c r="CE150" s="2"/>
       <c r="CF150" s="2"/>
     </row>
-    <row r="151" spans="1:84" ht="36">
+    <row r="151" spans="1:84" ht="24">
       <c r="A151" s="13" t="s">
         <v>569</v>
       </c>
@@ -14886,7 +14887,7 @@
       <c r="CE153" s="2"/>
       <c r="CF153" s="2"/>
     </row>
-    <row r="154" spans="1:84" ht="48">
+    <row r="154" spans="1:84" ht="36">
       <c r="A154" s="11" t="s">
         <v>581</v>
       </c>
@@ -14952,7 +14953,7 @@
       <c r="CE154" s="2"/>
       <c r="CF154" s="2"/>
     </row>
-    <row r="155" spans="1:84" ht="24">
+    <row r="155" spans="1:84">
       <c r="A155" s="11" t="s">
         <v>585</v>
       </c>
@@ -15014,7 +15015,7 @@
       <c r="CE155" s="2"/>
       <c r="CF155" s="2"/>
     </row>
-    <row r="156" spans="1:84" ht="24">
+    <row r="156" spans="1:84">
       <c r="A156" s="11" t="s">
         <v>588</v>
       </c>
@@ -15207,7 +15208,7 @@
       <c r="CE158" s="2"/>
       <c r="CF158" s="2"/>
     </row>
-    <row r="159" spans="1:84" ht="48">
+    <row r="159" spans="1:84" ht="36">
       <c r="A159" s="13" t="s">
         <v>598</v>
       </c>
@@ -15339,7 +15340,7 @@
       <c r="CE160" s="2"/>
       <c r="CF160" s="2"/>
     </row>
-    <row r="161" spans="1:84" ht="60">
+    <row r="161" spans="1:84" ht="48">
       <c r="A161" s="11" t="s">
         <v>605</v>
       </c>
@@ -15470,7 +15471,7 @@
       <c r="CE162" s="2"/>
       <c r="CF162" s="2"/>
     </row>
-    <row r="163" spans="1:84" ht="96">
+    <row r="163" spans="1:84" ht="84">
       <c r="A163" s="1" t="s">
         <v>611</v>
       </c>
@@ -15502,7 +15503,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="164" spans="1:84" ht="36">
+    <row r="164" spans="1:84" ht="24">
       <c r="A164" s="11" t="s">
         <v>614</v>
       </c>
@@ -15560,7 +15561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:84" ht="96">
+    <row r="165" spans="1:84" ht="72">
       <c r="A165" s="11" t="s">
         <v>617</v>
       </c>
@@ -15684,7 +15685,7 @@
       <c r="CE166" s="2"/>
       <c r="CF166" s="2"/>
     </row>
-    <row r="167" spans="1:84" ht="60">
+    <row r="167" spans="1:84" ht="48">
       <c r="A167" s="13" t="s">
         <v>626</v>
       </c>
@@ -15920,7 +15921,7 @@
       <c r="CE169" s="2"/>
       <c r="CF169" s="2"/>
     </row>
-    <row r="170" spans="1:84" ht="60">
+    <row r="170" spans="1:84" ht="48">
       <c r="A170" s="1" t="s">
         <v>639</v>
       </c>
@@ -16016,7 +16017,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="173" spans="1:84" ht="48">
+    <row r="173" spans="1:84" ht="36">
       <c r="A173" s="11" t="s">
         <v>648</v>
       </c>
@@ -16051,7 +16052,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="174" spans="1:84" ht="72">
+    <row r="174" spans="1:84" ht="48">
       <c r="A174" s="13" t="s">
         <v>651</v>
       </c>
@@ -16516,7 +16517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:84" ht="36">
+    <row r="181" spans="1:84" ht="24">
       <c r="A181" s="11" t="s">
         <v>678</v>
       </c>
@@ -16833,7 +16834,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="187" spans="1:84" ht="72">
+    <row r="187" spans="1:84" ht="60">
       <c r="A187" s="11" t="s">
         <v>698</v>
       </c>
@@ -17091,7 +17092,7 @@
       <c r="CE190" s="2"/>
       <c r="CF190" s="2"/>
     </row>
-    <row r="191" spans="1:84" ht="36">
+    <row r="191" spans="1:84" ht="24">
       <c r="A191" s="1" t="s">
         <v>713</v>
       </c>
@@ -17259,7 +17260,7 @@
       <c r="CE193" s="2"/>
       <c r="CF193" s="2"/>
     </row>
-    <row r="194" spans="1:84" ht="36">
+    <row r="194" spans="1:84" ht="24">
       <c r="A194" s="11" t="s">
         <v>722</v>
       </c>
@@ -17565,7 +17566,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="199" spans="1:84" ht="72">
+    <row r="199" spans="1:84" ht="60">
       <c r="A199" s="13" t="s">
         <v>737</v>
       </c>
@@ -18171,7 +18172,7 @@
       <c r="CE207" s="2"/>
       <c r="CF207" s="2"/>
     </row>
-    <row r="208" spans="1:84" ht="72">
+    <row r="208" spans="1:84" ht="60">
       <c r="A208" s="11" t="s">
         <v>764</v>
       </c>
@@ -18258,7 +18259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:84" ht="108">
+    <row r="210" spans="1:84" ht="96">
       <c r="A210" s="11" t="s">
         <v>770</v>
       </c>
@@ -18409,7 +18410,7 @@
       <c r="CE211" s="2"/>
       <c r="CF211" s="2"/>
     </row>
-    <row r="212" spans="1:84" ht="84">
+    <row r="212" spans="1:84" ht="72">
       <c r="A212" s="11" t="s">
         <v>777</v>
       </c>
@@ -18620,7 +18621,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="215" spans="1:84" ht="72">
+    <row r="215" spans="1:84" ht="60">
       <c r="A215" s="13" t="s">
         <v>789</v>
       </c>
@@ -18707,7 +18708,7 @@
       <c r="CE215" s="2"/>
       <c r="CF215" s="2"/>
     </row>
-    <row r="216" spans="1:84" ht="36">
+    <row r="216" spans="1:84" ht="24">
       <c r="A216" s="11" t="s">
         <v>793</v>
       </c>
@@ -18910,7 +18911,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="219" spans="1:84" ht="36">
+    <row r="219" spans="1:84" ht="24">
       <c r="A219" s="13" t="s">
         <v>805</v>
       </c>
@@ -19204,7 +19205,7 @@
       <c r="CE222" s="2"/>
       <c r="CF222" s="2"/>
     </row>
-    <row r="223" spans="1:84" ht="36">
+    <row r="223" spans="1:84" ht="24">
       <c r="A223" s="11" t="s">
         <v>820</v>
       </c>
@@ -19718,7 +19719,7 @@
       <c r="CE228" s="2"/>
       <c r="CF228" s="2"/>
     </row>
-    <row r="229" spans="1:84" ht="24">
+    <row r="229" spans="1:84">
       <c r="A229" s="13" t="s">
         <v>844</v>
       </c>
@@ -19869,7 +19870,7 @@
       <c r="CE230" s="2"/>
       <c r="CF230" s="2"/>
     </row>
-    <row r="231" spans="1:84" ht="60">
+    <row r="231" spans="1:84" ht="36">
       <c r="A231" s="11" t="s">
         <v>853</v>
       </c>
@@ -20062,7 +20063,7 @@
       <c r="CE233" s="2"/>
       <c r="CF233" s="2"/>
     </row>
-    <row r="234" spans="1:84" ht="48">
+    <row r="234" spans="1:84" ht="36">
       <c r="A234" s="11" t="s">
         <v>864</v>
       </c>
@@ -20235,7 +20236,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="237" spans="1:84" ht="36">
+    <row r="237" spans="1:84" ht="24">
       <c r="A237" s="11" t="s">
         <v>874</v>
       </c>
@@ -20299,7 +20300,7 @@
       <c r="CE237" s="2"/>
       <c r="CF237" s="2"/>
     </row>
-    <row r="238" spans="1:84" ht="48">
+    <row r="238" spans="1:84" ht="36">
       <c r="A238" s="13" t="s">
         <v>877</v>
       </c>
@@ -20560,10 +20561,10 @@
         <v>892</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D242" s="13">
         <v>3</v>
@@ -20798,7 +20799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:84" ht="48">
+    <row r="247" spans="1:84" ht="36">
       <c r="A247" s="13" t="s">
         <v>909</v>
       </c>
@@ -20855,7 +20856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:84" ht="36">
+    <row r="248" spans="1:84" ht="24">
       <c r="A248" s="11" t="s">
         <v>913</v>
       </c>
@@ -20973,7 +20974,7 @@
       <c r="CE249" s="2"/>
       <c r="CF249" s="2"/>
     </row>
-    <row r="250" spans="1:84" ht="84">
+    <row r="250" spans="1:84" ht="60">
       <c r="A250" s="11" t="s">
         <v>919</v>
       </c>
@@ -21121,7 +21122,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="253" spans="1:84" ht="84">
+    <row r="253" spans="1:84" ht="120">
       <c r="A253" s="11" t="s">
         <v>929</v>
       </c>
@@ -21148,10 +21149,10 @@
       <c r="J253" s="11"/>
       <c r="K253" s="11"/>
       <c r="L253" s="11" t="s">
-        <v>931</v>
+        <v>1248</v>
       </c>
       <c r="M253" s="14" t="s">
-        <v>932</v>
+        <v>1249</v>
       </c>
       <c r="U253" s="1">
         <f t="shared" ref="U253:Z254" si="79">IF(AA$1&gt;=$D253,$O253+$P253*($Q253+1)/2+$R253*($S253+1)/2*(AA$1-$D253),0)</f>
@@ -21188,7 +21189,7 @@
     </row>
     <row r="254" spans="1:84" ht="24">
       <c r="A254" s="11" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>848</v>
@@ -21206,7 +21207,7 @@
         <v>29</v>
       </c>
       <c r="G254" s="11" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="H254" s="11" t="s">
         <v>103</v>
@@ -21215,7 +21216,7 @@
       <c r="J254" s="11"/>
       <c r="K254" s="11"/>
       <c r="L254" s="11" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="U254" s="1">
         <f t="shared" si="79"/>
@@ -21244,7 +21245,7 @@
     </row>
     <row r="255" spans="1:84" ht="48">
       <c r="A255" s="11" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>848</v>
@@ -21262,7 +21263,7 @@
         <v>88</v>
       </c>
       <c r="G255" s="11" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="H255" s="11" t="s">
         <v>653</v>
@@ -21271,10 +21272,10 @@
       <c r="J255" s="11"/>
       <c r="K255" s="11"/>
       <c r="L255" s="11" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="M255" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="BF255" s="1"/>
       <c r="BG255" s="1"/>
@@ -21285,9 +21286,9 @@
       <c r="CE255" s="2"/>
       <c r="CF255" s="2"/>
     </row>
-    <row r="256" spans="1:84" ht="48">
+    <row r="256" spans="1:84" ht="36">
       <c r="A256" s="11" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>848</v>
@@ -21305,10 +21306,10 @@
         <v>35</v>
       </c>
       <c r="G256" s="11" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H256" s="11" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="I256" s="11"/>
       <c r="J256" s="11"/>
@@ -21316,10 +21317,10 @@
         <v>68</v>
       </c>
       <c r="L256" s="11" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="M256" s="14" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="N256" s="1">
         <v>1</v>
@@ -21372,9 +21373,9 @@
       <c r="CE256" s="2"/>
       <c r="CF256" s="2"/>
     </row>
-    <row r="257" spans="1:84" ht="72">
+    <row r="257" spans="1:84" ht="60">
       <c r="A257" s="11" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>848</v>
@@ -21392,14 +21393,14 @@
         <v>29</v>
       </c>
       <c r="G257" s="11" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H257" s="11"/>
       <c r="I257" s="11"/>
       <c r="J257" s="11"/>
       <c r="K257" s="11"/>
       <c r="L257" s="11" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="M257" s="12"/>
       <c r="U257" s="1">
@@ -21435,9 +21436,9 @@
       <c r="CE257" s="2"/>
       <c r="CF257" s="2"/>
     </row>
-    <row r="258" spans="1:84" ht="60">
+    <row r="258" spans="1:84" ht="48">
       <c r="A258" s="11" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>848</v>
@@ -21455,7 +21456,7 @@
         <v>29</v>
       </c>
       <c r="G258" s="11" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H258" s="11" t="s">
         <v>344</v>
@@ -21466,7 +21467,7 @@
         <v>137</v>
       </c>
       <c r="L258" s="11" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="U258" s="1">
         <f t="shared" si="80"/>
@@ -21503,7 +21504,7 @@
     </row>
     <row r="259" spans="1:84" ht="36">
       <c r="A259" s="11" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>848</v>
@@ -21521,17 +21522,17 @@
         <v>29</v>
       </c>
       <c r="G259" s="11" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="H259" s="15"/>
       <c r="I259" s="11"/>
       <c r="J259" s="11"/>
       <c r="K259" s="11"/>
       <c r="L259" s="11" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="M259" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="U259" s="1">
         <f t="shared" si="80"/>
@@ -21568,7 +21569,7 @@
     </row>
     <row r="260" spans="1:84" ht="24">
       <c r="A260" s="11" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>848</v>
@@ -21586,7 +21587,7 @@
         <v>29</v>
       </c>
       <c r="G260" s="11" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="H260" s="11" t="s">
         <v>103</v>
@@ -21595,7 +21596,7 @@
       <c r="J260" s="11"/>
       <c r="K260" s="11"/>
       <c r="L260" s="11" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="U260" s="1">
         <f t="shared" si="80"/>
@@ -21630,9 +21631,9 @@
       <c r="CE260" s="2"/>
       <c r="CF260" s="2"/>
     </row>
-    <row r="261" spans="1:84" ht="48">
+    <row r="261" spans="1:84" ht="36">
       <c r="A261" s="11" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>848</v>
@@ -21650,19 +21651,19 @@
         <v>29</v>
       </c>
       <c r="G261" s="11" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="H261" s="11" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="I261" s="11"/>
       <c r="J261" s="11"/>
       <c r="K261" s="11"/>
       <c r="L261" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="M261" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="U261" s="1">
         <f t="shared" si="80"/>
@@ -21697,9 +21698,9 @@
       <c r="CE261" s="2"/>
       <c r="CF261" s="2"/>
     </row>
-    <row r="262" spans="1:84" ht="48">
+    <row r="262" spans="1:84" ht="36">
       <c r="A262" s="11" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>848</v>
@@ -21717,19 +21718,19 @@
         <v>29</v>
       </c>
       <c r="G262" s="11" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="H262" s="11" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="I262" s="11"/>
       <c r="J262" s="11"/>
       <c r="K262" s="11"/>
       <c r="L262" s="11" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="M262" s="14" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="U262" s="1">
         <f t="shared" si="80"/>
@@ -21766,7 +21767,7 @@
     </row>
     <row r="263" spans="1:84" ht="72">
       <c r="A263" s="11" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>848</v>
@@ -21784,7 +21785,7 @@
         <v>29</v>
       </c>
       <c r="G263" s="11" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="H263" s="11" t="s">
         <v>273</v>
@@ -21795,10 +21796,10 @@
         <v>116</v>
       </c>
       <c r="L263" s="11" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="M263" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="N263" s="1">
         <v>1</v>
@@ -21853,7 +21854,7 @@
     </row>
     <row r="264" spans="1:84" ht="60">
       <c r="A264" s="11" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>848</v>
@@ -21871,7 +21872,7 @@
         <v>35</v>
       </c>
       <c r="G264" s="11" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="H264" s="11" t="s">
         <v>107</v>
@@ -21880,10 +21881,10 @@
       <c r="J264" s="11"/>
       <c r="K264" s="11"/>
       <c r="L264" s="11" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="M264" s="14" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="U264" s="1">
         <f t="shared" si="80"/>
@@ -21920,7 +21921,7 @@
     </row>
     <row r="265" spans="1:84" ht="36">
       <c r="A265" s="11" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>848</v>
@@ -21938,7 +21939,7 @@
         <v>83</v>
       </c>
       <c r="G265" s="11" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="H265" s="11" t="s">
         <v>593</v>
@@ -21947,10 +21948,10 @@
       <c r="J265" s="11"/>
       <c r="K265" s="11"/>
       <c r="L265" s="11" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="M265" s="14" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="U265" s="1">
         <f t="shared" si="80"/>
@@ -21987,7 +21988,7 @@
     </row>
     <row r="266" spans="1:84" ht="24">
       <c r="A266" s="11" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>848</v>
@@ -22005,7 +22006,7 @@
         <v>29</v>
       </c>
       <c r="G266" s="11" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="H266" s="11" t="s">
         <v>273</v>
@@ -22014,7 +22015,7 @@
       <c r="J266" s="11"/>
       <c r="K266" s="11"/>
       <c r="L266" s="11" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="U266" s="1">
         <f t="shared" si="80"/>
@@ -22049,9 +22050,9 @@
       <c r="CE266" s="2"/>
       <c r="CF266" s="2"/>
     </row>
-    <row r="267" spans="1:84" ht="84">
+    <row r="267" spans="1:84" ht="72">
       <c r="A267" s="11" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>848</v>
@@ -22069,7 +22070,7 @@
         <v>29</v>
       </c>
       <c r="G267" s="11" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="H267" s="11" t="s">
         <v>344</v>
@@ -22078,7 +22079,7 @@
       <c r="J267" s="11"/>
       <c r="K267" s="11"/>
       <c r="L267" s="11" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="U267" s="1">
         <f t="shared" si="80"/>
@@ -22115,7 +22116,7 @@
     </row>
     <row r="268" spans="1:84" ht="48">
       <c r="A268" s="11" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>848</v>
@@ -22133,17 +22134,17 @@
         <v>29</v>
       </c>
       <c r="G268" s="11" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="H268" s="11"/>
       <c r="I268" s="11"/>
       <c r="J268" s="11"/>
       <c r="K268" s="11"/>
       <c r="L268" s="11" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M268" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="U268" s="1">
         <f t="shared" si="80"/>
@@ -22180,7 +22181,7 @@
     </row>
     <row r="269" spans="1:84" ht="36">
       <c r="A269" s="11" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>848</v>
@@ -22198,7 +22199,7 @@
         <v>29</v>
       </c>
       <c r="G269" s="11" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="H269" s="11" t="s">
         <v>344</v>
@@ -22207,10 +22208,10 @@
       <c r="J269" s="11"/>
       <c r="K269" s="11"/>
       <c r="L269" s="11" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="M269" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="U269" s="1">
         <f t="shared" si="80"/>
@@ -22245,9 +22246,9 @@
       <c r="CE269" s="2"/>
       <c r="CF269" s="2"/>
     </row>
-    <row r="270" spans="1:84" ht="72">
+    <row r="270" spans="1:84" ht="60">
       <c r="A270" s="11" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>848</v>
@@ -22265,7 +22266,7 @@
         <v>35</v>
       </c>
       <c r="G270" s="11" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="H270" s="11"/>
       <c r="I270" s="11"/>
@@ -22274,10 +22275,10 @@
         <v>859</v>
       </c>
       <c r="L270" s="11" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="M270" s="14" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="U270" s="1">
         <f t="shared" si="80"/>
@@ -22312,9 +22313,9 @@
       <c r="CE270" s="2"/>
       <c r="CF270" s="2"/>
     </row>
-    <row r="271" spans="1:84" ht="180">
+    <row r="271" spans="1:84" ht="156">
       <c r="A271" s="11" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>848</v>
@@ -22326,20 +22327,20 @@
         <v>6</v>
       </c>
       <c r="E271" s="11" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F271" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G271" s="11" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="H271" s="11"/>
       <c r="I271" s="11"/>
       <c r="J271" s="11"/>
       <c r="K271" s="11"/>
       <c r="L271" s="11" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="U271" s="1">
         <f t="shared" si="80"/>
@@ -22376,13 +22377,13 @@
     </row>
     <row r="272" spans="1:84" ht="24">
       <c r="A272" s="11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C272" s="11" t="s">
         <v>1002</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C272" s="11" t="s">
-        <v>1004</v>
       </c>
       <c r="D272" s="20">
         <v>1</v>
@@ -22394,7 +22395,7 @@
         <v>35</v>
       </c>
       <c r="G272" s="11" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="H272" s="11" t="s">
         <v>434</v>
@@ -22403,7 +22404,7 @@
       <c r="J272" s="20"/>
       <c r="K272" s="20"/>
       <c r="L272" s="11" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="M272" s="12"/>
       <c r="U272" s="1">
@@ -22431,15 +22432,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:125" ht="60">
+    <row r="273" spans="1:125" ht="48">
       <c r="A273" s="11" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C273" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D273" s="20">
         <v>1</v>
@@ -22451,7 +22452,7 @@
         <v>88</v>
       </c>
       <c r="G273" s="11" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="H273" s="11" t="s">
         <v>344</v>
@@ -22460,7 +22461,7 @@
       <c r="J273" s="20"/>
       <c r="K273" s="20"/>
       <c r="L273" s="11" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="M273" s="12"/>
       <c r="U273" s="1">
@@ -22496,15 +22497,15 @@
       <c r="CE273" s="2"/>
       <c r="CF273" s="2"/>
     </row>
-    <row r="274" spans="1:125" ht="36">
+    <row r="274" spans="1:125" ht="24">
       <c r="A274" s="11" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C274" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D274" s="20">
         <v>1</v>
@@ -22516,7 +22517,7 @@
         <v>83</v>
       </c>
       <c r="G274" s="11" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
@@ -22525,7 +22526,7 @@
         <v>68</v>
       </c>
       <c r="L274" s="11" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="U274" s="1">
         <f t="shared" si="80"/>
@@ -22562,13 +22563,13 @@
     </row>
     <row r="275" spans="1:125" ht="24">
       <c r="A275" s="11" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C275" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D275" s="11">
         <v>1</v>
@@ -22580,14 +22581,14 @@
         <v>29</v>
       </c>
       <c r="G275" s="11" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="H275" s="11"/>
       <c r="I275" s="11"/>
       <c r="J275" s="11"/>
       <c r="K275" s="11"/>
       <c r="L275" s="11" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="U275" s="1">
         <f t="shared" si="80"/>
@@ -22622,15 +22623,15 @@
       <c r="CE275" s="2"/>
       <c r="CF275" s="2"/>
     </row>
-    <row r="276" spans="1:125" ht="72">
+    <row r="276" spans="1:125" ht="60">
       <c r="A276" s="11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C276" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D276" s="20">
         <v>1</v>
@@ -22642,7 +22643,7 @@
         <v>35</v>
       </c>
       <c r="G276" s="11" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="H276" s="11" t="s">
         <v>103</v>
@@ -22653,10 +22654,10 @@
         <v>232</v>
       </c>
       <c r="L276" s="11" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M276" s="1" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="U276" s="1">
         <f t="shared" si="80"/>
@@ -22691,15 +22692,15 @@
       <c r="CE276" s="2"/>
       <c r="CF276" s="2"/>
     </row>
-    <row r="277" spans="1:125" ht="96">
+    <row r="277" spans="1:125" ht="84">
       <c r="A277" s="11" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C277" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D277" s="20">
         <v>2</v>
@@ -22711,17 +22712,17 @@
         <v>35</v>
       </c>
       <c r="G277" s="11" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="H277" s="20"/>
       <c r="I277" s="20"/>
       <c r="J277" s="20"/>
       <c r="K277" s="20"/>
       <c r="L277" s="11" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="M277" s="1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="U277" s="1">
         <f t="shared" si="80"/>
@@ -22758,13 +22759,13 @@
     </row>
     <row r="278" spans="1:125" ht="24">
       <c r="A278" s="11" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C278" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D278" s="20">
         <v>2</v>
@@ -22776,7 +22777,7 @@
         <v>35</v>
       </c>
       <c r="G278" s="11" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="H278" s="11" t="s">
         <v>434</v>
@@ -22785,7 +22786,7 @@
       <c r="J278" s="20"/>
       <c r="K278" s="20"/>
       <c r="L278" s="11" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="M278" s="12"/>
       <c r="U278" s="1">
@@ -22824,13 +22825,13 @@
     </row>
     <row r="279" spans="1:125" ht="48">
       <c r="A279" s="11" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C279" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D279" s="11">
         <v>2</v>
@@ -22842,7 +22843,7 @@
         <v>29</v>
       </c>
       <c r="G279" s="11" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="H279" s="11" t="s">
         <v>213</v>
@@ -22851,10 +22852,10 @@
       <c r="J279" s="11"/>
       <c r="K279" s="11"/>
       <c r="L279" s="11" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="M279" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="U279" s="1">
         <f t="shared" si="80"/>
@@ -22891,13 +22892,13 @@
     </row>
     <row r="280" spans="1:125" ht="24">
       <c r="A280" s="11" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C280" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D280" s="20">
         <v>2</v>
@@ -22909,7 +22910,7 @@
         <v>35</v>
       </c>
       <c r="G280" s="11" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H280" s="11" t="s">
         <v>267</v>
@@ -22920,10 +22921,10 @@
         <v>137</v>
       </c>
       <c r="L280" s="11" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="M280" s="12" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="U280" s="1">
         <f t="shared" si="80"/>
@@ -22960,13 +22961,13 @@
     </row>
     <row r="281" spans="1:125" ht="72">
       <c r="A281" s="11" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C281" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D281" s="20">
         <v>3</v>
@@ -22978,7 +22979,7 @@
         <v>35</v>
       </c>
       <c r="G281" s="11" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="H281" s="11" t="s">
         <v>103</v>
@@ -22987,7 +22988,7 @@
       <c r="J281" s="20"/>
       <c r="K281" s="20"/>
       <c r="L281" s="11" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="M281" s="12"/>
       <c r="U281" s="1">
@@ -23023,15 +23024,15 @@
       <c r="CE281" s="2"/>
       <c r="CF281" s="2"/>
     </row>
-    <row r="282" spans="1:125" ht="84">
+    <row r="282" spans="1:125" ht="72">
       <c r="A282" s="11" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C282" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D282" s="20">
         <v>3</v>
@@ -23043,7 +23044,7 @@
         <v>35</v>
       </c>
       <c r="G282" s="11" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="H282" s="11" t="s">
         <v>213</v>
@@ -23054,7 +23055,7 @@
         <v>232</v>
       </c>
       <c r="L282" s="11" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="M282" s="12"/>
       <c r="U282" s="1">
@@ -23092,13 +23093,13 @@
     </row>
     <row r="283" spans="1:125" ht="36">
       <c r="A283" s="11" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C283" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D283" s="11">
         <v>3</v>
@@ -23110,7 +23111,7 @@
         <v>29</v>
       </c>
       <c r="G283" s="11" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="H283" s="11" t="s">
         <v>103</v>
@@ -23119,7 +23120,7 @@
       <c r="J283" s="11"/>
       <c r="K283" s="11"/>
       <c r="L283" s="11" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="M283" s="12"/>
       <c r="U283" s="1">
@@ -23157,13 +23158,13 @@
     </row>
     <row r="284" spans="1:125" ht="24">
       <c r="A284" s="11" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C284" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D284" s="11">
         <v>3</v>
@@ -23175,7 +23176,7 @@
         <v>35</v>
       </c>
       <c r="G284" s="11" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="H284" s="11" t="s">
         <v>103</v>
@@ -23184,7 +23185,7 @@
       <c r="J284" s="11"/>
       <c r="K284" s="11"/>
       <c r="L284" s="11" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="M284" s="12"/>
       <c r="U284" s="1">
@@ -23222,13 +23223,13 @@
     </row>
     <row r="285" spans="1:125" ht="24">
       <c r="A285" s="11" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C285" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D285" s="20">
         <v>3</v>
@@ -23240,14 +23241,14 @@
         <v>35</v>
       </c>
       <c r="G285" s="11" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="H285" s="20"/>
       <c r="I285" s="20"/>
       <c r="J285" s="20"/>
       <c r="K285" s="20"/>
       <c r="L285" s="11" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="M285" s="12"/>
       <c r="U285" s="1">
@@ -23285,13 +23286,13 @@
     </row>
     <row r="286" spans="1:125" ht="24">
       <c r="A286" s="11" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C286" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D286" s="20">
         <v>4</v>
@@ -23303,7 +23304,7 @@
         <v>35</v>
       </c>
       <c r="G286" s="11" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H286" s="11" t="s">
         <v>454</v>
@@ -23312,7 +23313,7 @@
       <c r="J286" s="20"/>
       <c r="K286" s="20"/>
       <c r="L286" s="11" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="M286" s="12"/>
       <c r="U286" s="1">
@@ -23348,15 +23349,15 @@
       <c r="CE286" s="2"/>
       <c r="CF286" s="2"/>
     </row>
-    <row r="287" spans="1:125" ht="48">
+    <row r="287" spans="1:125" ht="36">
       <c r="A287" s="11" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C287" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D287" s="20">
         <v>2</v>
@@ -23368,14 +23369,14 @@
         <v>35</v>
       </c>
       <c r="G287" s="11" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="H287" s="20"/>
       <c r="I287" s="20"/>
       <c r="J287" s="20"/>
       <c r="K287" s="20"/>
       <c r="L287" s="11" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="M287" s="12"/>
       <c r="U287" s="1">
@@ -23413,13 +23414,13 @@
     </row>
     <row r="288" spans="1:125" ht="24">
       <c r="A288" s="11" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C288" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D288" s="20">
         <v>4</v>
@@ -23431,7 +23432,7 @@
         <v>35</v>
       </c>
       <c r="G288" s="11" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="H288" s="11" t="s">
         <v>103</v>
@@ -23440,10 +23441,10 @@
       <c r="J288" s="20"/>
       <c r="K288" s="20"/>
       <c r="L288" s="11" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="M288" s="1" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="U288" s="1">
         <f t="shared" ref="U288:U311" si="86">IF(AA$1&gt;=$D288,$O288+$P288*($Q288+1)/2+$R288*($S288+1)/2*(AA$1-$D288),0)</f>
@@ -23480,13 +23481,13 @@
     </row>
     <row r="289" spans="1:84" ht="24">
       <c r="A289" s="11" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C289" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D289" s="11">
         <v>4</v>
@@ -23498,19 +23499,19 @@
         <v>29</v>
       </c>
       <c r="G289" s="11" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="H289" s="11" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="I289" s="11"/>
       <c r="J289" s="11"/>
       <c r="K289" s="11"/>
       <c r="L289" s="11" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="M289" s="12" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="U289" s="1">
         <f t="shared" si="86"/>
@@ -23545,15 +23546,15 @@
       <c r="CE289" s="2"/>
       <c r="CF289" s="2"/>
     </row>
-    <row r="290" spans="1:84" ht="72">
+    <row r="290" spans="1:84" ht="60">
       <c r="A290" s="11" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C290" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D290" s="20">
         <v>5</v>
@@ -23565,14 +23566,14 @@
         <v>35</v>
       </c>
       <c r="G290" s="11" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
       <c r="J290" s="20"/>
       <c r="K290" s="20"/>
       <c r="L290" s="11" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="U290" s="1">
         <f t="shared" si="86"/>
@@ -23599,15 +23600,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:84" ht="168">
+    <row r="291" spans="1:84" ht="144">
       <c r="A291" s="11" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C291" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D291" s="20">
         <v>5</v>
@@ -23619,14 +23620,14 @@
         <v>88</v>
       </c>
       <c r="G291" s="11" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
       <c r="J291" s="20"/>
       <c r="K291" s="20"/>
       <c r="L291" s="11" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="M291" s="12"/>
       <c r="U291" s="1">
@@ -23664,13 +23665,13 @@
     </row>
     <row r="292" spans="1:84" ht="24">
       <c r="A292" s="11" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C292" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D292" s="20">
         <v>6</v>
@@ -23682,7 +23683,7 @@
         <v>35</v>
       </c>
       <c r="G292" s="11" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="H292" s="11" t="s">
         <v>344</v>
@@ -23691,7 +23692,7 @@
       <c r="J292" s="20"/>
       <c r="K292" s="20"/>
       <c r="L292" s="11" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="M292" s="12"/>
       <c r="U292" s="1">
@@ -23727,15 +23728,15 @@
       <c r="CE292" s="2"/>
       <c r="CF292" s="2"/>
     </row>
-    <row r="293" spans="1:84" ht="36">
+    <row r="293" spans="1:84" ht="24">
       <c r="A293" s="11" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C293" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D293" s="20">
         <v>1</v>
@@ -23747,7 +23748,7 @@
         <v>29</v>
       </c>
       <c r="G293" s="11" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="H293" s="11" t="s">
         <v>527</v>
@@ -23756,7 +23757,7 @@
       <c r="J293" s="20"/>
       <c r="K293" s="20"/>
       <c r="L293" s="11" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="M293" s="12"/>
       <c r="U293" s="1">
@@ -23792,15 +23793,15 @@
       <c r="CE293" s="2"/>
       <c r="CF293" s="2"/>
     </row>
-    <row r="294" spans="1:84" ht="60">
+    <row r="294" spans="1:84" ht="48">
       <c r="A294" s="11" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C294" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D294" s="20">
         <v>1</v>
@@ -23812,7 +23813,7 @@
         <v>35</v>
       </c>
       <c r="G294" s="11" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="H294" s="20"/>
       <c r="I294" s="20" t="s">
@@ -23823,10 +23824,10 @@
       </c>
       <c r="K294" s="11"/>
       <c r="L294" s="11" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="M294" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="N294" s="1">
         <v>1</v>
@@ -23879,15 +23880,15 @@
       <c r="CE294" s="2"/>
       <c r="CF294" s="2"/>
     </row>
-    <row r="295" spans="1:84" ht="36">
+    <row r="295" spans="1:84" ht="24">
       <c r="A295" s="11" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C295" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D295" s="11">
         <v>1</v>
@@ -23899,7 +23900,7 @@
         <v>35</v>
       </c>
       <c r="G295" s="11" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="H295" s="11" t="s">
         <v>107</v>
@@ -23912,7 +23913,7 @@
       </c>
       <c r="K295" s="11"/>
       <c r="L295" s="11" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="U295" s="1">
         <f t="shared" si="86"/>
@@ -23939,15 +23940,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:84" ht="36">
+    <row r="296" spans="1:84" ht="24">
       <c r="A296" s="11" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C296" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D296" s="20">
         <v>1</v>
@@ -23959,10 +23960,10 @@
         <v>35</v>
       </c>
       <c r="G296" s="11" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="H296" s="11" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="I296" s="20"/>
       <c r="J296" s="20"/>
@@ -23970,7 +23971,7 @@
         <v>583</v>
       </c>
       <c r="L296" s="11" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="M296" s="12"/>
       <c r="U296" s="1">
@@ -24006,15 +24007,15 @@
       <c r="CE296" s="2"/>
       <c r="CF296" s="2"/>
     </row>
-    <row r="297" spans="1:84" ht="72">
+    <row r="297" spans="1:84" ht="60">
       <c r="A297" s="11" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C297" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D297" s="20">
         <v>1</v>
@@ -24026,7 +24027,7 @@
         <v>29</v>
       </c>
       <c r="G297" s="11" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="H297" s="11" t="s">
         <v>103</v>
@@ -24035,10 +24036,10 @@
       <c r="J297" s="20"/>
       <c r="K297" s="20"/>
       <c r="L297" s="11" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="M297" s="18" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="U297" s="1">
         <f t="shared" si="86"/>
@@ -24075,13 +24076,13 @@
     </row>
     <row r="298" spans="1:84" ht="48">
       <c r="A298" s="11" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C298" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D298" s="11">
         <v>2</v>
@@ -24093,7 +24094,7 @@
         <v>35</v>
       </c>
       <c r="G298" s="11" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="H298" s="11" t="s">
         <v>653</v>
@@ -24102,7 +24103,7 @@
       <c r="J298" s="11"/>
       <c r="K298" s="11"/>
       <c r="L298" s="11" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="M298" s="12"/>
       <c r="U298" s="1">
@@ -24140,13 +24141,13 @@
     </row>
     <row r="299" spans="1:84" ht="36">
       <c r="A299" s="11" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C299" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D299" s="20">
         <v>2</v>
@@ -24158,7 +24159,7 @@
         <v>35</v>
       </c>
       <c r="G299" s="11" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="H299" s="11" t="s">
         <v>103</v>
@@ -24167,10 +24168,10 @@
       <c r="J299" s="20"/>
       <c r="K299" s="20"/>
       <c r="L299" s="11" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="M299" s="12" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="U299" s="1">
         <f t="shared" si="86"/>
@@ -24205,15 +24206,15 @@
       <c r="CE299" s="2"/>
       <c r="CF299" s="2"/>
     </row>
-    <row r="300" spans="1:84" ht="48">
+    <row r="300" spans="1:84" ht="36">
       <c r="A300" s="11" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C300" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D300" s="20">
         <v>2</v>
@@ -24225,16 +24226,16 @@
         <v>29</v>
       </c>
       <c r="G300" s="11" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="H300" s="11" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="I300" s="20"/>
       <c r="J300" s="20"/>
       <c r="K300" s="20"/>
       <c r="L300" s="11" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="M300" s="12"/>
       <c r="U300" s="1">
@@ -24272,13 +24273,13 @@
     </row>
     <row r="301" spans="1:84" ht="24">
       <c r="A301" s="11" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C301" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D301" s="20">
         <v>2</v>
@@ -24290,7 +24291,7 @@
         <v>29</v>
       </c>
       <c r="G301" s="11" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="H301" s="11" t="s">
         <v>90</v>
@@ -24299,10 +24300,10 @@
       <c r="J301" s="20"/>
       <c r="K301" s="20"/>
       <c r="L301" s="11" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="M301" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="U301" s="1">
         <f t="shared" si="86"/>
@@ -24339,13 +24340,13 @@
     </row>
     <row r="302" spans="1:84" ht="48">
       <c r="A302" s="11" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C302" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D302" s="20">
         <v>3</v>
@@ -24357,7 +24358,7 @@
         <v>35</v>
       </c>
       <c r="G302" s="11" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="H302" s="11" t="s">
         <v>213</v>
@@ -24368,7 +24369,7 @@
         <v>42</v>
       </c>
       <c r="L302" s="11" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="M302" s="12"/>
       <c r="U302" s="1">
@@ -24404,15 +24405,15 @@
       <c r="CE302" s="2"/>
       <c r="CF302" s="2"/>
     </row>
-    <row r="303" spans="1:84" ht="120">
+    <row r="303" spans="1:84" ht="96">
       <c r="A303" s="11" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C303" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D303" s="20">
         <v>3</v>
@@ -24424,19 +24425,19 @@
         <v>35</v>
       </c>
       <c r="G303" s="11" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="H303" s="11" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="I303" s="20"/>
       <c r="J303" s="20"/>
       <c r="K303" s="20"/>
       <c r="L303" s="11" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="M303" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="U303" s="1">
         <f t="shared" si="86"/>
@@ -24473,13 +24474,13 @@
     </row>
     <row r="304" spans="1:84" ht="60">
       <c r="A304" s="11" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C304" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D304" s="20">
         <v>3</v>
@@ -24491,7 +24492,7 @@
         <v>35</v>
       </c>
       <c r="G304" s="11" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="H304" s="11" t="s">
         <v>107</v>
@@ -24504,10 +24505,10 @@
       </c>
       <c r="K304" s="20"/>
       <c r="L304" s="11" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="M304" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="N304" s="1">
         <v>1</v>
@@ -24560,15 +24561,15 @@
       <c r="CE304" s="2"/>
       <c r="CF304" s="2"/>
     </row>
-    <row r="305" spans="1:84" ht="36">
+    <row r="305" spans="1:84" ht="24">
       <c r="A305" s="11" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C305" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D305" s="20">
         <v>3</v>
@@ -24580,7 +24581,7 @@
         <v>35</v>
       </c>
       <c r="G305" s="11" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="H305" s="20"/>
       <c r="I305" s="20"/>
@@ -24589,10 +24590,10 @@
         <v>232</v>
       </c>
       <c r="L305" s="11" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="M305" s="1" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="U305" s="1">
         <f t="shared" si="86"/>
@@ -24629,13 +24630,13 @@
     </row>
     <row r="306" spans="1:84" ht="36">
       <c r="A306" s="11" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C306" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D306" s="20">
         <v>4</v>
@@ -24647,7 +24648,7 @@
         <v>83</v>
       </c>
       <c r="G306" s="11" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="H306" s="20"/>
       <c r="I306" s="20"/>
@@ -24656,7 +24657,7 @@
         <v>232</v>
       </c>
       <c r="L306" s="11" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="M306" s="12"/>
       <c r="U306" s="1">
@@ -24694,13 +24695,13 @@
     </row>
     <row r="307" spans="1:84" ht="24">
       <c r="A307" s="11" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C307" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D307" s="20">
         <v>4</v>
@@ -24712,7 +24713,7 @@
         <v>29</v>
       </c>
       <c r="G307" s="11" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="H307" s="11" t="s">
         <v>624</v>
@@ -24721,7 +24722,7 @@
       <c r="J307" s="20"/>
       <c r="K307" s="20"/>
       <c r="L307" s="11" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="M307" s="12"/>
       <c r="U307" s="1">
@@ -24759,13 +24760,13 @@
     </row>
     <row r="308" spans="1:84" ht="36">
       <c r="A308" s="11" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C308" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D308" s="20">
         <v>4</v>
@@ -24777,7 +24778,7 @@
         <v>35</v>
       </c>
       <c r="G308" s="11" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="H308" s="20"/>
       <c r="I308" s="20" t="s">
@@ -24788,10 +24789,10 @@
       </c>
       <c r="K308" s="11"/>
       <c r="L308" s="11" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="M308" s="12" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="N308" s="1">
         <v>1</v>
@@ -24844,15 +24845,15 @@
       <c r="CE308" s="2"/>
       <c r="CF308" s="2"/>
     </row>
-    <row r="309" spans="1:84" ht="192">
+    <row r="309" spans="1:84" ht="168">
       <c r="A309" s="11" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C309" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D309" s="20">
         <v>5</v>
@@ -24864,7 +24865,7 @@
         <v>29</v>
       </c>
       <c r="G309" s="11" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="H309" s="20" t="s">
         <v>273</v>
@@ -24873,7 +24874,7 @@
       <c r="J309" s="20"/>
       <c r="K309" s="20"/>
       <c r="L309" s="11" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="U309" s="1">
         <f t="shared" si="86"/>
@@ -24900,15 +24901,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:84" ht="108">
+    <row r="310" spans="1:84" ht="84">
       <c r="A310" s="11" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C310" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D310" s="20">
         <v>5</v>
@@ -24920,7 +24921,7 @@
         <v>88</v>
       </c>
       <c r="G310" s="11" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="H310" s="11" t="s">
         <v>344</v>
@@ -24931,7 +24932,7 @@
         <v>232</v>
       </c>
       <c r="L310" s="11" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="M310" s="12"/>
       <c r="U310" s="1">
@@ -24961,13 +24962,13 @@
     </row>
     <row r="311" spans="1:84" ht="84">
       <c r="A311" s="11" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C311" s="11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D311" s="20">
         <v>6</v>
@@ -24979,7 +24980,7 @@
         <v>88</v>
       </c>
       <c r="G311" s="11" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="H311" s="11" t="s">
         <v>344</v>
@@ -24988,7 +24989,7 @@
       <c r="J311" s="20"/>
       <c r="K311" s="20"/>
       <c r="L311" s="11" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="M311" s="12"/>
       <c r="U311" s="1">
@@ -25018,13 +25019,13 @@
     </row>
     <row r="312" spans="1:84" ht="108">
       <c r="A312" s="1" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D312" s="1">
         <v>2</v>
@@ -25036,27 +25037,27 @@
         <v>88</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>267</v>
       </c>
       <c r="L312" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="M312" s="1" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="313" spans="1:84" ht="132">
       <c r="A313" s="1" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D313" s="1">
         <v>6</v>
@@ -25068,18 +25069,18 @@
         <v>35</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="K313" s="1" t="s">
         <v>232</v>
       </c>
       <c r="L313" s="1" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="314" spans="1:84" ht="60">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="314" spans="1:84" ht="48">
       <c r="A314" s="1" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>570</v>
@@ -25097,7 +25098,7 @@
         <v>29</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>439</v>
@@ -25106,12 +25107,12 @@
         <v>859</v>
       </c>
       <c r="L314" s="1" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="315" spans="1:84" ht="48">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="315" spans="1:84" ht="36">
       <c r="A315" s="1" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>848</v>
@@ -25129,18 +25130,18 @@
         <v>29</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>344</v>
       </c>
       <c r="L315" s="1" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="316" spans="1:84" ht="204">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="316" spans="1:84" ht="192">
       <c r="A316" s="1" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>296</v>
@@ -25161,12 +25162,12 @@
         <v>515</v>
       </c>
       <c r="L316" s="1" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="317" spans="1:84" ht="132">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="317" spans="1:84" ht="120">
       <c r="A317" s="1" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>419</v>
@@ -25178,7 +25179,7 @@
         <v>6</v>
       </c>
       <c r="E317" s="1" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="F317" s="1" t="s">
         <v>88</v>
@@ -25187,12 +25188,12 @@
         <v>273</v>
       </c>
       <c r="L317" s="1" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="318" spans="1:84" ht="108">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="318" spans="1:84" ht="96">
       <c r="A318" s="1" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>570</v>
@@ -25210,7 +25211,7 @@
         <v>29</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>103</v>
@@ -25219,12 +25220,12 @@
         <v>116</v>
       </c>
       <c r="L318" s="1" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="319" spans="1:84" ht="72">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="319" spans="1:84" ht="60">
       <c r="A319" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>570</v>
@@ -25242,21 +25243,21 @@
         <v>29</v>
       </c>
       <c r="G319" s="22" t="s">
+        <v>1162</v>
+      </c>
+      <c r="H319" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="L319" s="1" t="s">
         <v>1164</v>
       </c>
-      <c r="H319" s="1" t="s">
+      <c r="M319" s="1" t="s">
         <v>1165</v>
-      </c>
-      <c r="L319" s="1" t="s">
-        <v>1166</v>
-      </c>
-      <c r="M319" s="1" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="320" spans="1:84" ht="108">
       <c r="A320" s="1" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>570</v>
@@ -25274,18 +25275,18 @@
         <v>35</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="K320" s="1" t="s">
         <v>515</v>
       </c>
       <c r="L320" s="1" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="321" spans="1:13" ht="108">
       <c r="A321" s="1" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>570</v>
@@ -25303,21 +25304,21 @@
         <v>29</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="H321" s="1" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="K321" s="1" t="s">
         <v>620</v>
       </c>
       <c r="L321" s="1" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="322" spans="1:13" ht="60">
       <c r="A322" s="1" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>570</v>
@@ -25335,18 +25336,18 @@
         <v>35</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="K322" s="1" t="s">
         <v>300</v>
       </c>
       <c r="L322" s="1" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="323" spans="1:13" ht="84">
       <c r="A323" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>705</v>
@@ -25364,7 +25365,7 @@
         <v>35</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>344</v>
@@ -25379,12 +25380,12 @@
         <v>68</v>
       </c>
       <c r="L323" s="1" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="324" spans="1:13" ht="48">
       <c r="A324" s="1" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>705</v>
@@ -25402,24 +25403,24 @@
         <v>35</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>267</v>
       </c>
       <c r="K324" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="L324" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="M324" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="L324" s="1" t="s">
+    </row>
+    <row r="325" spans="1:13" ht="60">
+      <c r="A325" s="1" t="s">
         <v>1183</v>
-      </c>
-      <c r="M324" s="1" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="325" spans="1:13" ht="72">
-      <c r="A325" s="1" t="s">
-        <v>1185</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>705</v>
@@ -25437,21 +25438,21 @@
         <v>35</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="H325" s="1" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="K325" s="1" t="s">
         <v>131</v>
       </c>
       <c r="L325" s="1" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="326" spans="1:13" ht="60">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" ht="48">
       <c r="A326" s="1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>705</v>
@@ -25469,7 +25470,7 @@
         <v>35</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="H326" s="1" t="s">
         <v>267</v>
@@ -25478,12 +25479,12 @@
         <v>232</v>
       </c>
       <c r="L326" s="1" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="327" spans="1:13" ht="24">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13">
       <c r="A327" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>848</v>
@@ -25501,18 +25502,18 @@
         <v>35</v>
       </c>
       <c r="G327" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="L327" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="M327" s="1" t="s">
         <v>1193</v>
-      </c>
-      <c r="L327" s="1" t="s">
-        <v>1194</v>
-      </c>
-      <c r="M327" s="1" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="328" spans="1:13" ht="120">
       <c r="A328" s="1" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>848</v>
@@ -25530,7 +25531,7 @@
         <v>29</v>
       </c>
       <c r="G328" s="1" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="H328" s="1" t="s">
         <v>213</v>
@@ -25539,12 +25540,12 @@
         <v>116</v>
       </c>
       <c r="L328" s="1" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="329" spans="1:13" ht="252">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" ht="228">
       <c r="A329" s="1" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>705</v>
@@ -25562,7 +25563,7 @@
         <v>83</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="H329" s="1" t="s">
         <v>267</v>
@@ -25571,12 +25572,12 @@
         <v>232</v>
       </c>
       <c r="L329" s="1" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="330" spans="1:13" ht="48">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" ht="36">
       <c r="A330" s="1" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>705</v>
@@ -25594,18 +25595,18 @@
         <v>35</v>
       </c>
       <c r="G330" s="1" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="K330" s="1" t="s">
         <v>42</v>
       </c>
       <c r="L330" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="331" spans="1:13" ht="48">
       <c r="A331" s="1" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>705</v>
@@ -25623,21 +25624,21 @@
         <v>35</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="K331" s="1" t="s">
         <v>68</v>
       </c>
       <c r="L331" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="M331" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="332" spans="1:13" ht="48">
       <c r="A332" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>296</v>
@@ -25655,7 +25656,7 @@
         <v>35</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="I332" s="1" t="s">
         <v>37</v>
@@ -25664,15 +25665,15 @@
         <v>300</v>
       </c>
       <c r="L332" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="M332" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="333" spans="1:13" ht="48">
       <c r="A333" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>296</v>
@@ -25690,18 +25691,18 @@
         <v>29</v>
       </c>
       <c r="H333" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="K333" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="L333" s="1" t="s">
         <v>1213</v>
-      </c>
-      <c r="K333" s="1" t="s">
-        <v>1214</v>
-      </c>
-      <c r="L333" s="1" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="334" spans="1:13" ht="96">
       <c r="A334" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>296</v>
@@ -25719,15 +25720,15 @@
         <v>88</v>
       </c>
       <c r="H334" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="L334" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="335" spans="1:13" ht="72">
       <c r="A335" s="1" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>705</v>
@@ -25745,16 +25746,16 @@
         <v>35</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="H335" s="1" t="s">
         <v>665</v>
       </c>
       <c r="K335" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="L335" s="1" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="M335" s="1" t="s">
         <v>819</v>
@@ -25762,7 +25763,7 @@
     </row>
     <row r="336" spans="1:13" ht="72">
       <c r="A336" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>705</v>
@@ -25780,18 +25781,18 @@
         <v>35</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="I336" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L336" s="1" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="48">
       <c r="A337" s="1" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>848</v>
@@ -25809,18 +25810,18 @@
         <v>29</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="H337" s="1" t="s">
         <v>103</v>
       </c>
       <c r="L337" s="1" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="48">
       <c r="A338" s="1" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>848</v>
@@ -25838,21 +25839,21 @@
         <v>35</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="H338" s="1" t="s">
         <v>213</v>
       </c>
       <c r="L338" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="M338" s="1" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" ht="144">
+      <c r="A339" s="1" t="s">
         <v>1232</v>
-      </c>
-      <c r="M338" s="1" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="339" spans="1:13" ht="156">
-      <c r="A339" s="1" t="s">
-        <v>1234</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>26</v>
@@ -25870,24 +25871,24 @@
         <v>88</v>
       </c>
       <c r="G339" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H339" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L339" s="1" t="s">
         <v>1236</v>
-      </c>
-      <c r="H339" s="1" t="s">
-        <v>1237</v>
-      </c>
-      <c r="L339" s="1" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="252">
       <c r="A340" s="1" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D340" s="1">
         <v>1</v>
@@ -25899,27 +25900,27 @@
         <v>35</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="H340" s="1" t="s">
         <v>267</v>
       </c>
       <c r="L340" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="M340" s="1" t="s">
         <v>1244</v>
-      </c>
-      <c r="M340" s="1" t="s">
-        <v>1246</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="252">
       <c r="A341" s="1" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D341" s="1">
         <v>1</v>
@@ -25931,7 +25932,7 @@
         <v>35</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="H341" s="1" t="s">
         <v>267</v>
@@ -25940,15 +25941,15 @@
         <v>232</v>
       </c>
       <c r="L341" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="M341" s="1" t="s">
         <v>1245</v>
-      </c>
-      <c r="M341" s="1" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="36">
       <c r="A342" s="1" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>419</v>
@@ -25966,28 +25967,18 @@
         <v>35</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="K342" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="L342" s="1" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:EP311" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="19">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
     <mergeCell ref="CE1:CE2"/>
     <mergeCell ref="DB1:DU1"/>
     <mergeCell ref="DW1:EP1"/>
@@ -25997,6 +25988,16 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="CC1:CC2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
HUGE CHANGE. REVERT TO ONE BEFORE HER TO RECOVER
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/AllSpells.xlsx
+++ b/CoreRulebook/Data/Spells/AllSpells.xlsx
@@ -1238,7 +1238,7 @@
     <t xml:space="preserve">A beam of light causes the target\apos{}s muscles to atrophy and their mind to cloud for an instant, before the effect wears off. The target must deduct 1d4 from the value of their next check. </t>
   </si>
   <si>
-    <t xml:space="preserve">Palpatation</t>
+    <t xml:space="preserve">Palpitation</t>
   </si>
   <si>
     <t xml:space="preserve">vena</t>
@@ -2411,7 +2411,7 @@
     <t xml:space="preserve">A wave of energy strikes into the target, causing 1d6 force damage, and if the target fails to Resist, pushing the target backwards up to 1 metre. </t>
   </si>
   <si>
-    <t xml:space="preserve">Each additional casting level dedicated to this spell increases the power of the energy-wave: do an additional 1d8 force damage and push the target back an extra 2 metres. </t>
+    <t xml:space="preserve">Each additional casting level dedicated to this spell increases the power of the energy-wave: do an additional 1d6 force damage and push the target back an extra 2 metres. </t>
   </si>
   <si>
     <t xml:space="preserve">Magnetising Strike</t>
@@ -5149,11 +5149,11 @@
   <dimension ref="A1:FK385"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E357" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="L179" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A357" activeCellId="0" sqref="A357"/>
-      <selection pane="bottomRight" activeCell="E361" activeCellId="0" sqref="E361"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A179" activeCellId="0" sqref="A179"/>
+      <selection pane="bottomRight" activeCell="L183" activeCellId="0" sqref="L183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>